<commit_message>
version 2.3 - Capped DPT score at 100
</commit_message>
<xml_diff>
--- a/external/country-averages-Pan.xlsx
+++ b/external/country-averages-Pan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d4a9fd65a6bad53/Seun/2. Career and business/3. IQVIA-Asiwaju-PC/Analysis/tHFA/external/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{A5C4C092-52B6-44A6-A6F9-F06C09FDB8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08B6D089-A958-490E-8479-2CE7D2CBFDE1}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{A5C4C092-52B6-44A6-A6F9-F06C09FDB8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A163521-B5D2-495E-8424-3C6BE8F4C1A4}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="0" windowWidth="16320" windowHeight="10800" xr2:uid="{553B10A4-C7F2-48F3-85E4-2CA0E02AF682}"/>
+    <workbookView xWindow="1140" yWindow="0" windowWidth="16320" windowHeight="10800" xr2:uid="{553B10A4-C7F2-48F3-85E4-2CA0E02AF682}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -550,7 +550,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -760,7 +760,7 @@
         <v>26.280380000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -924,7 +924,7 @@
         <v>15.66667</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1148,7 +1148,7 @@
   <autoFilter ref="A1:M14" xr:uid="{577EBEB3-AF04-449C-AFC2-4CE0CA425D6F}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Ghana"/>
+        <filter val="Malawi"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>